<commit_message>
🧹 Cleanup: Remove backup files
</commit_message>
<xml_diff>
--- a/data/user_credentials_export.xlsx
+++ b/data/user_credentials_export.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/praveenchaudhary/Downloads/Agent/followup-reminder-agent/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460C804A-8E80-D644-A9AB-298A7BBA5315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="76">
   <si>
     <t>username</t>
   </si>
@@ -131,9 +137,6 @@
   </si>
   <si>
     <t>Nupur Munjal</t>
-  </si>
-  <si>
-    <t>admin@koenig-solutions.com</t>
   </si>
   <si>
     <t>Sunilkumar.kushwaha@koenig-solutions.com</t>
@@ -250,8 +253,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,13 +317,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -358,7 +369,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -392,6 +403,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -426,9 +438,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -601,14 +614,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -639,22 +658,22 @@
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -662,22 +681,22 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -685,22 +704,22 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -708,22 +727,22 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -731,22 +750,22 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -754,22 +773,22 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -777,22 +796,22 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -800,22 +819,22 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -823,22 +842,22 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -846,22 +865,22 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -869,22 +888,22 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -892,22 +911,22 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -915,22 +934,22 @@
         <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -938,22 +957,22 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -961,22 +980,22 @@
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -984,19 +1003,19 @@
         <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>